<commit_message>
Update the input sheet by clinet needed
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389F56F2-8B31-8B42-BB2F-5C320D60B9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B9477-EF83-6A45-BAB9-7D09369F7ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="175">
   <si>
     <t>Timestamp</t>
   </si>
@@ -81,18 +81,6 @@
     <t>M/W/F schedule [5:45 - 6:35 p.m.]</t>
   </si>
   <si>
-    <t>M/W schedule [9:05 - 10:20 a.m.]</t>
-  </si>
-  <si>
-    <t>M/W schedule [11:15  - 12:30 p.m.]</t>
-  </si>
-  <si>
-    <t>M/W schedule [1:25 - 2:40 p.m.]</t>
-  </si>
-  <si>
-    <t>M/W schedule [3:35 - 4:40 p.m.]</t>
-  </si>
-  <si>
     <t>T/TH schedule [8:00 - 9:15 a.m.]</t>
   </si>
   <si>
@@ -553,6 +541,21 @@
   </si>
   <si>
     <t>Raghavendra</t>
+  </si>
+  <si>
+    <t>M/W schedule [8:05 - 9:15 a.m.]</t>
+  </si>
+  <si>
+    <t>M/W schedule [10:10 - 11:25 a.m.]</t>
+  </si>
+  <si>
+    <t>M/W schedule [12:20 - 1:35 p.m.]</t>
+  </si>
+  <si>
+    <t>M/W schedule [2:30 - 3:45 p.m.]</t>
+  </si>
+  <si>
+    <t>M/W schedule [4:40 - 5:55 p.m.]</t>
   </si>
 </sst>
 </file>
@@ -1409,29 +1412,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="107" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y21" sqref="J21:Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="16" max="16" width="24.83203125" customWidth="1"/>
-    <col min="17" max="17" width="29" customWidth="1"/>
-    <col min="18" max="18" width="26.83203125" customWidth="1"/>
-    <col min="19" max="19" width="22.6640625" customWidth="1"/>
-    <col min="20" max="20" width="22" customWidth="1"/>
-    <col min="21" max="21" width="26.33203125" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" customWidth="1"/>
-    <col min="24" max="24" width="17.6640625" customWidth="1"/>
-    <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="26" max="26" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="37.1640625" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="16" max="16" width="30.5" customWidth="1"/>
+    <col min="17" max="17" width="32.5" customWidth="1"/>
+    <col min="18" max="18" width="29" customWidth="1"/>
+    <col min="19" max="19" width="26.83203125" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="22" max="22" width="26.33203125" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.6640625" customWidth="1"/>
+    <col min="26" max="26" width="25" customWidth="1"/>
+    <col min="27" max="27" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1481,1110 +1487,1113 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" t="s">
+        <v>172</v>
+      </c>
+      <c r="T1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U1" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45748.569444444445</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45748.572222222225</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="W4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="W5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" t="s">
-        <v>30</v>
-      </c>
-      <c r="T6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="X7" t="s">
-        <v>30</v>
-      </c>
       <c r="Y7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>48</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="W8" t="s">
-        <v>30</v>
-      </c>
-      <c r="X8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="X11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="V10" t="s">
-        <v>30</v>
-      </c>
-      <c r="W10" t="s">
-        <v>30</v>
-      </c>
-      <c r="X10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="X12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="W11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D13" t="s">
         <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="W12" t="s">
-        <v>30</v>
-      </c>
-      <c r="X12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="Y14" t="s">
-        <v>30</v>
-      </c>
       <c r="Z14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="W16" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="AA17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="X19" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
         <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="W19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" t="s">
-        <v>85</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M22" t="s">
-        <v>30</v>
-      </c>
-      <c r="W22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="X22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="V24" t="s">
+        <v>26</v>
+      </c>
+      <c r="W24" t="s">
+        <v>26</v>
+      </c>
+      <c r="X24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>96</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="U24" t="s">
-        <v>30</v>
-      </c>
-      <c r="V24" t="s">
-        <v>30</v>
-      </c>
-      <c r="W24" t="s">
-        <v>30</v>
-      </c>
-      <c r="X24" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="O25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
-      <c r="X27" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="X28" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="Y28" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="X29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
         <v>110</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D30" t="s">
         <v>111</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="V30" t="s">
+        <v>26</v>
+      </c>
+      <c r="W30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>112</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="W29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="C31" t="s">
         <v>113</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
         <v>114</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="U30" t="s">
-        <v>30</v>
-      </c>
-      <c r="V30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="V32" t="s">
+        <v>26</v>
+      </c>
+      <c r="W32" t="s">
+        <v>26</v>
+      </c>
+      <c r="X32" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>120</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="W33" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>121</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="U32" t="s">
-        <v>30</v>
-      </c>
-      <c r="V32" t="s">
-        <v>30</v>
-      </c>
-      <c r="W32" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>122</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D34" t="s">
         <v>123</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="W34" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>124</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="V33" t="s">
-        <v>30</v>
-      </c>
-      <c r="W33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>125</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
         <v>126</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="X35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>127</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="V34" t="s">
-        <v>30</v>
-      </c>
-      <c r="X34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>128</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D36" t="s">
         <v>129</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>130</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="W35" t="s">
-        <v>30</v>
-      </c>
-      <c r="X35" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>131</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D37" t="s">
         <v>132</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="W37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>133</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="X36" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>134</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
         <v>135</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="V38" t="s">
+        <v>26</v>
+      </c>
+      <c r="W38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>136</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="V37" t="s">
-        <v>30</v>
-      </c>
-      <c r="X37" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="C39" t="s">
         <v>137</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" t="s">
         <v>138</v>
-      </c>
-      <c r="D38" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="U38" t="s">
-        <v>30</v>
-      </c>
-      <c r="V38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" t="s">
-        <v>142</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
-      <c r="U40" t="s">
-        <v>30</v>
-      </c>
       <c r="V40" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="W40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="X40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
         <v>145</v>
-      </c>
-      <c r="C41" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" t="s">
-        <v>30</v>
-      </c>
-      <c r="J41" t="s">
-        <v>30</v>
-      </c>
-      <c r="K41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" t="s">
-        <v>149</v>
       </c>
       <c r="E42">
         <v>2</v>
       </c>
-      <c r="W42" t="s">
-        <v>30</v>
-      </c>
       <c r="X42" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Y42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" t="s">
+        <v>148</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="X43" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" t="s">
         <v>150</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>151</v>
-      </c>
-      <c r="D43" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="W43" t="s">
-        <v>30</v>
-      </c>
-      <c r="X43" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" t="s">
-        <v>154</v>
-      </c>
-      <c r="D44" t="s">
-        <v>155</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="W44" t="s">
-        <v>30</v>
-      </c>
       <c r="X44" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Y44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="W45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" t="s">
         <v>156</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>157</v>
-      </c>
-      <c r="D45" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="V45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" t="s">
-        <v>160</v>
-      </c>
-      <c r="D46" t="s">
-        <v>161</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
-      <c r="U46" t="s">
-        <v>30</v>
-      </c>
-      <c r="W46" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="V46" t="s">
+        <v>26</v>
+      </c>
+      <c r="X46" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
       </c>
-      <c r="R47" t="s">
-        <v>30</v>
-      </c>
       <c r="S47" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="T47" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="U47" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E48" s="2">
         <v>1</v>
       </c>
-      <c r="AA48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AB48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
+        <v>26</v>
+      </c>
+      <c r="S49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>165</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>164</v>
       </c>
-      <c r="E49" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>30</v>
-      </c>
-      <c r="R49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
+      <c r="U51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
         <v>167</v>
       </c>
-      <c r="C50" t="s">
-        <v>166</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C51" t="s">
-        <v>168</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
-      <c r="T51" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C52" t="s">
-        <v>171</v>
-      </c>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:26" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>172</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="E53" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Extract facultys time preference csv
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B9477-EF83-6A45-BAB9-7D09369F7ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67024754-CBAB-7F4B-B458-7E6EFC262F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="175">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1414,14 +1414,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="J21:Y21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="75" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="37.1640625" customWidth="1"/>
     <col min="8" max="8" width="27.83203125" customWidth="1"/>
     <col min="16" max="16" width="30.5" customWidth="1"/>
@@ -2587,6 +2588,24 @@
       <c r="E52" s="2">
         <v>1</v>
       </c>
+      <c r="I52" t="s">
+        <v>26</v>
+      </c>
+      <c r="J52" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" t="s">
+        <v>26</v>
+      </c>
+      <c r="R52" t="s">
+        <v>26</v>
+      </c>
+      <c r="S52" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="53" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
@@ -2597,6 +2616,9 @@
       </c>
       <c r="E53" s="2">
         <v>1</v>
+      </c>
+      <c r="T53" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove dupilicate professor from input
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74801537-5A93-2041-BB84-47268825D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44697303-A0F2-6649-A948-CB38E16378C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="177">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1418,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB54"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="Z54" sqref="Z54"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:AJ53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,7 +2216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>118</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>121</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>124</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>127</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>130</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>133</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>136</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>139</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>141</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>144</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>146</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>149</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>152</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>155</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>159</v>
       </c>
@@ -2540,46 +2540,49 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="E48" s="2">
         <v>1</v>
       </c>
-      <c r="AB48" t="s">
+      <c r="R48" t="s">
+        <v>26</v>
+      </c>
+      <c r="S48" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E49" s="2">
         <v>1</v>
       </c>
-      <c r="R49" t="s">
-        <v>26</v>
-      </c>
-      <c r="S49" t="s">
+      <c r="AA49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="50" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E50" s="2">
         <v>1</v>
+      </c>
+      <c r="U50" t="s">
+        <v>26</v>
       </c>
       <c r="AA50" t="s">
         <v>26</v>
@@ -2587,75 +2590,58 @@
     </row>
     <row r="51" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C51" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E51" s="2">
         <v>1</v>
       </c>
-      <c r="U51" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>26</v>
+      </c>
+      <c r="J51" t="s">
+        <v>26</v>
+      </c>
+      <c r="K51" t="s">
+        <v>26</v>
+      </c>
+      <c r="L51" t="s">
+        <v>26</v>
+      </c>
+      <c r="R51" t="s">
+        <v>26</v>
+      </c>
+      <c r="S51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="E52" s="2">
         <v>1</v>
       </c>
-      <c r="I52" t="s">
-        <v>26</v>
-      </c>
-      <c r="J52" t="s">
-        <v>26</v>
-      </c>
-      <c r="K52" t="s">
-        <v>26</v>
-      </c>
-      <c r="L52" t="s">
-        <v>26</v>
-      </c>
-      <c r="R52" t="s">
-        <v>26</v>
-      </c>
-      <c r="S52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="T52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>168</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
+      </c>
+      <c r="C53" t="s">
+        <v>176</v>
       </c>
       <c r="E53" s="2">
         <v>1</v>
       </c>
-      <c r="T53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z54" t="s">
+      <c r="Z53" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Kandel Jade's time
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44697303-A0F2-6649-A948-CB38E16378C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501A77A6-4092-F942-9230-7008235CFA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="177">
   <si>
     <t>Timestamp</t>
   </si>
@@ -513,12 +513,6 @@
     <t>Ryan</t>
   </si>
   <si>
-    <t>Mingyu</t>
-  </si>
-  <si>
-    <t>Ding</t>
-  </si>
-  <si>
     <t>Julia</t>
   </si>
   <si>
@@ -562,6 +556,12 @@
   </si>
   <si>
     <t>tianlong</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>Kandel</t>
   </si>
 </sst>
 </file>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:AJ53"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1431,6 +1431,7 @@
     <col min="6" max="6" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="37.1640625" customWidth="1"/>
     <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="13" max="13" width="27.1640625" customWidth="1"/>
     <col min="16" max="16" width="30.5" customWidth="1"/>
     <col min="17" max="17" width="32.5" customWidth="1"/>
     <col min="18" max="18" width="29" customWidth="1"/>
@@ -1494,19 +1495,19 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R1" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" t="s">
         <v>170</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>171</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>172</v>
-      </c>
-      <c r="T1" t="s">
-        <v>173</v>
-      </c>
-      <c r="U1" t="s">
-        <v>174</v>
       </c>
       <c r="V1" t="s">
         <v>16</v>
@@ -1763,7 +1764,7 @@
         <v>54</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X11" t="s">
         <v>26</v>
@@ -1912,7 +1913,7 @@
         <v>75</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.2">
@@ -2550,10 +2551,7 @@
       <c r="E48" s="2">
         <v>1</v>
       </c>
-      <c r="R48" t="s">
-        <v>26</v>
-      </c>
-      <c r="S48" t="s">
+      <c r="AA48" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2567,81 +2565,81 @@
       <c r="E49" s="2">
         <v>1</v>
       </c>
+      <c r="U49" t="s">
+        <v>26</v>
+      </c>
       <c r="AA49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="50" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" t="s">
         <v>165</v>
       </c>
-      <c r="C50" t="s">
-        <v>164</v>
-      </c>
       <c r="E50" s="2">
         <v>1</v>
       </c>
-      <c r="U50" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" t="s">
+        <v>26</v>
+      </c>
+      <c r="K50" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" t="s">
+        <v>26</v>
+      </c>
+      <c r="R50" t="s">
+        <v>26</v>
+      </c>
+      <c r="S50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:27" ht="18" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>166</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
         <v>167</v>
       </c>
       <c r="E51" s="2">
         <v>1</v>
       </c>
-      <c r="I51" t="s">
-        <v>26</v>
-      </c>
-      <c r="J51" t="s">
-        <v>26</v>
-      </c>
-      <c r="K51" t="s">
-        <v>26</v>
-      </c>
-      <c r="L51" t="s">
-        <v>26</v>
-      </c>
-      <c r="R51" t="s">
-        <v>26</v>
-      </c>
-      <c r="S51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="T51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>168</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="C52" t="s">
+        <v>174</v>
       </c>
       <c r="E52" s="2">
         <v>1</v>
       </c>
-      <c r="T52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+      <c r="Z52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
         <v>175</v>
       </c>
-      <c r="C53" t="s">
-        <v>176</v>
-      </c>
       <c r="E53" s="2">
         <v>1</v>
       </c>
-      <c r="Z53" t="s">
+      <c r="T53" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fill time for Kaur
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501A77A6-4092-F942-9230-7008235CFA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701311C1-1D5E-7D49-8D86-7EF82AE8BBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="177">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="93" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1915,6 +1915,9 @@
       <c r="E18">
         <v>2</v>
       </c>
+      <c r="X18" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19" t="s">

</xml_diff>

<commit_message>
Rename the output file
</commit_message>
<xml_diff>
--- a/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
+++ b/data/Input/Temple of Automatic course scheduling data sheet (Responses) - Form Responses 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD7A6A2-03BB-6B45-AF12-C3E8206A93D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AD0C1B-3AE2-2541-AE01-F0B5B768A354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="181">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L35" zoomScale="114" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="114" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2118,7 +2118,10 @@
         <v>99</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="X26" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.2">

</xml_diff>